<commit_message>
récupère les autres semaines
</commit_message>
<xml_diff>
--- a/SAE_3_01/Documents/QuiFaitQuoi_beta.xlsx
+++ b/SAE_3_01/Documents/QuiFaitQuoi_beta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chihebbradai/Documents/GitHub/SAE-3.01/SAE_3_01/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7AA161-7F55-9A41-9814-0D3F323E20EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA8F044-B96D-5547-BBEC-0CD0DD151366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>Ressource</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>R2.06</t>
+  </si>
+  <si>
+    <t>IIIIII</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1080,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1215,7 +1218,9 @@
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:10" ht="14" x14ac:dyDescent="0.15">
-      <c r="B8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F8">
         <v>1</v>
       </c>

</xml_diff>